<commit_message>
replaced soil_sns frontend with SN74
</commit_message>
<xml_diff>
--- a/SproutSync-Pin-Mapping-Petal-Ecosystem.xlsx
+++ b/SproutSync-Pin-Mapping-Petal-Ecosystem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjswe/Greenhouse/Hardware/SensorNode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2211927F-3ACD-1B4F-B270-A3C988759784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02EF36D7-7BF2-CD47-BCE0-E79760E227AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="25360" windowHeight="26260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30240" yWindow="9900" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apollo3 Pin Functions" sheetId="24" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="578">
   <si>
     <t>A1</t>
   </si>
@@ -1751,21 +1751,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>SENS_IO5,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFAA21D5"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> WIFI_TX_PETAL_RX1</t>
-    </r>
-  </si>
-  <si>
     <t>UART_TX</t>
   </si>
   <si>
@@ -1799,9 +1784,6 @@
     <t>WRT_ENA</t>
   </si>
   <si>
-    <t>SERIAL_OE</t>
-  </si>
-  <si>
     <t>AMB_SNS_ENA</t>
   </si>
   <si>
@@ -1812,15 +1794,34 @@
   </si>
   <si>
     <t>IRRI_ENA</t>
+  </si>
+  <si>
+    <t>RESERVE_GPIO*</t>
+  </si>
+  <si>
+    <t>USER_LED</t>
+  </si>
+  <si>
+    <t>SWCLK</t>
+  </si>
+  <si>
+    <t>nLORA_EN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1993,7 +1994,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2185,6 +2186,12 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="44">
     <border>
@@ -2744,11 +2751,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -2788,11 +2796,11 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -2804,95 +2812,95 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2905,88 +2913,88 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2998,28 +3006,28 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3037,7 +3045,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3058,134 +3066,134 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="43" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
@@ -3204,26 +3212,26 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -3250,9 +3258,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -3262,68 +3267,86 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" xfId="1" applyProtection="1">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" xfId="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3342,65 +3365,54 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="2" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -3416,36 +3428,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3502,33 +3484,10 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="0" tint="-0.24994659260841701"/>
       </font>
       <fill>
         <patternFill>
-          <fgColor theme="0" tint="-4.9989318521683403E-2"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -3545,12 +3504,41 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0" tint="-0.14996795556505021"/>
+        <color theme="1" tint="0.34998626667073579"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
+        <patternFill patternType="lightUp">
+          <fgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3628,21 +3616,13 @@
       <font>
         <b/>
         <i val="0"/>
+        <color theme="0"/>
       </font>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor theme="3"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3651,6 +3631,38 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4106,7 +4118,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4155,38 +4167,38 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="173" t="s">
+      <c r="N1" s="196" t="s">
         <v>268</v>
       </c>
-      <c r="O1" s="174"/>
-      <c r="P1" s="174"/>
-      <c r="Q1" s="174"/>
-      <c r="R1" s="174"/>
-      <c r="S1" s="174"/>
-      <c r="T1" s="174"/>
-      <c r="U1" s="175"/>
+      <c r="O1" s="197"/>
+      <c r="P1" s="197"/>
+      <c r="Q1" s="197"/>
+      <c r="R1" s="197"/>
+      <c r="S1" s="197"/>
+      <c r="T1" s="197"/>
+      <c r="U1" s="198"/>
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
       <c r="X1" s="9"/>
-      <c r="Y1" s="192" t="s">
+      <c r="Y1" s="175" t="s">
         <v>446</v>
       </c>
-      <c r="Z1" s="193"/>
-      <c r="AA1" s="193"/>
-      <c r="AB1" s="194"/>
+      <c r="Z1" s="176"/>
+      <c r="AA1" s="176"/>
+      <c r="AB1" s="177"/>
       <c r="AC1" s="9"/>
-      <c r="AD1" s="197" t="s">
+      <c r="AD1" s="180" t="s">
         <v>504</v>
       </c>
-      <c r="AE1" s="198"/>
-      <c r="AG1" s="195" t="s">
+      <c r="AE1" s="181"/>
+      <c r="AG1" s="178" t="s">
         <v>503</v>
       </c>
-      <c r="AH1" s="196"/>
-      <c r="AI1" s="196"/>
-      <c r="AJ1" s="196"/>
-      <c r="AK1" s="196"/>
-      <c r="AL1" s="196"/>
+      <c r="AH1" s="179"/>
+      <c r="AI1" s="179"/>
+      <c r="AJ1" s="179"/>
+      <c r="AK1" s="179"/>
+      <c r="AL1" s="179"/>
       <c r="AM1" s="9"/>
       <c r="AN1" s="9"/>
       <c r="AO1" s="9"/>
@@ -4325,9 +4337,6 @@
       </c>
       <c r="E3" s="43" t="s">
         <v>315</v>
-      </c>
-      <c r="G3" s="172" t="s">
-        <v>570</v>
       </c>
       <c r="H3" s="43" t="str">
         <f t="shared" ref="H3:H34" si="0">IF(Q3="",E3,IF(J3="","",HLOOKUP(J3,$N$2:$U$56,ROW(J3)-1)))</f>
@@ -4399,12 +4408,12 @@
       <c r="AK3" s="94"/>
       <c r="AL3" s="95"/>
       <c r="AM3" s="9"/>
-      <c r="AN3" s="182" t="s">
+      <c r="AN3" s="204" t="s">
         <v>532</v>
       </c>
-      <c r="AO3" s="183"/>
-      <c r="AP3" s="183"/>
-      <c r="AQ3" s="184"/>
+      <c r="AO3" s="205"/>
+      <c r="AP3" s="205"/>
+      <c r="AQ3" s="206"/>
       <c r="AR3" s="9"/>
       <c r="AS3" s="48"/>
     </row>
@@ -4425,7 +4434,7 @@
         <v>310</v>
       </c>
       <c r="G4" s="172" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="H4" s="43" t="str">
         <f t="shared" si="0"/>
@@ -4499,11 +4508,11 @@
       <c r="AK4" s="94"/>
       <c r="AL4" s="95"/>
       <c r="AM4" s="9"/>
-      <c r="AN4" s="177" t="s">
+      <c r="AN4" s="199" t="s">
         <v>139</v>
       </c>
-      <c r="AO4" s="178"/>
-      <c r="AP4" s="179"/>
+      <c r="AO4" s="200"/>
+      <c r="AP4" s="201"/>
       <c r="AQ4" s="51" t="s">
         <v>262</v>
       </c>
@@ -4526,8 +4535,8 @@
       <c r="E5" s="43" t="s">
         <v>305</v>
       </c>
-      <c r="G5" s="156" t="s">
-        <v>559</v>
+      <c r="G5" s="172" t="s">
+        <v>572</v>
       </c>
       <c r="H5" s="43" t="str">
         <f t="shared" si="0"/>
@@ -4604,10 +4613,10 @@
       <c r="AN5" s="99" t="s">
         <v>168</v>
       </c>
-      <c r="AO5" s="180" t="s">
+      <c r="AO5" s="202" t="s">
         <v>140</v>
       </c>
-      <c r="AP5" s="180"/>
+      <c r="AP5" s="202"/>
       <c r="AQ5" s="4" t="s">
         <v>349</v>
       </c>
@@ -4630,7 +4639,9 @@
       <c r="E6" s="43" t="s">
         <v>311</v>
       </c>
-      <c r="G6" s="153"/>
+      <c r="G6" s="1" t="s">
+        <v>574</v>
+      </c>
       <c r="H6" s="43" t="str">
         <f t="shared" si="0"/>
         <v>GPIO03*</v>
@@ -4704,10 +4715,10 @@
       <c r="AN6" s="67" t="s">
         <v>166</v>
       </c>
-      <c r="AO6" s="181" t="s">
+      <c r="AO6" s="203" t="s">
         <v>141</v>
       </c>
-      <c r="AP6" s="181"/>
+      <c r="AP6" s="203"/>
       <c r="AQ6" s="5" t="s">
         <v>349</v>
       </c>
@@ -4730,7 +4741,9 @@
       <c r="E7" s="43" t="s">
         <v>298</v>
       </c>
-      <c r="G7" s="157"/>
+      <c r="G7" s="172" t="s">
+        <v>573</v>
+      </c>
       <c r="H7" s="43" t="str">
         <f t="shared" si="0"/>
         <v>GPIO04</v>
@@ -4818,10 +4831,10 @@
       <c r="AN7" s="100" t="s">
         <v>165</v>
       </c>
-      <c r="AO7" s="176" t="s">
+      <c r="AO7" s="174" t="s">
         <v>142</v>
       </c>
-      <c r="AP7" s="176"/>
+      <c r="AP7" s="174"/>
       <c r="AQ7" s="5" t="s">
         <v>349</v>
       </c>
@@ -4844,17 +4857,19 @@
       <c r="E8" s="43" t="s">
         <v>302</v>
       </c>
-      <c r="G8" s="156"/>
+      <c r="G8" s="172" t="s">
+        <v>565</v>
+      </c>
       <c r="H8" s="43" t="str">
         <f t="shared" si="0"/>
-        <v>M0SCK</v>
+        <v>GPIO05</v>
       </c>
       <c r="I8" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J8" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="9"/>
@@ -4932,10 +4947,10 @@
       <c r="AN8" s="101" t="s">
         <v>167</v>
       </c>
-      <c r="AO8" s="176" t="s">
+      <c r="AO8" s="174" t="s">
         <v>163</v>
       </c>
-      <c r="AP8" s="176"/>
+      <c r="AP8" s="174"/>
       <c r="AQ8" s="5" t="s">
         <v>349</v>
       </c>
@@ -4958,17 +4973,19 @@
       <c r="E9" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="G9" s="156"/>
+      <c r="G9" s="172" t="s">
+        <v>568</v>
+      </c>
       <c r="H9" s="43" t="str">
         <f t="shared" si="0"/>
-        <v>M0MISO</v>
+        <v>GPIO06</v>
       </c>
       <c r="I9" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J9" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="9"/>
@@ -5046,10 +5063,10 @@
       <c r="AN9" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="AO9" s="176" t="s">
+      <c r="AO9" s="174" t="s">
         <v>184</v>
       </c>
-      <c r="AP9" s="176"/>
+      <c r="AP9" s="174"/>
       <c r="AQ9" s="5" t="s">
         <v>349</v>
       </c>
@@ -5073,7 +5090,7 @@
         <v>307</v>
       </c>
       <c r="G10" s="172" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="H10" s="43" t="str">
         <f t="shared" si="0"/>
@@ -5162,10 +5179,10 @@
       <c r="AN10" s="102" t="s">
         <v>187</v>
       </c>
-      <c r="AO10" s="176" t="s">
+      <c r="AO10" s="174" t="s">
         <v>185</v>
       </c>
-      <c r="AP10" s="176"/>
+      <c r="AP10" s="174"/>
       <c r="AQ10" s="5" t="s">
         <v>349</v>
       </c>
@@ -5188,17 +5205,19 @@
       <c r="E11" s="43" t="s">
         <v>306</v>
       </c>
-      <c r="G11" s="156"/>
+      <c r="G11" s="172" t="s">
+        <v>571</v>
+      </c>
       <c r="H11" s="43" t="str">
         <f t="shared" si="0"/>
-        <v>M1SCL</v>
+        <v>GPIO08</v>
       </c>
       <c r="I11" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J11" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="9"/>
@@ -5262,10 +5281,10 @@
       <c r="AN11" s="103" t="s">
         <v>188</v>
       </c>
-      <c r="AO11" s="176" t="s">
+      <c r="AO11" s="174" t="s">
         <v>186</v>
       </c>
-      <c r="AP11" s="176"/>
+      <c r="AP11" s="174"/>
       <c r="AQ11" s="5" t="s">
         <v>349</v>
       </c>
@@ -5288,7 +5307,6 @@
       <c r="E12" s="43" t="s">
         <v>312</v>
       </c>
-      <c r="G12" s="156"/>
       <c r="H12" s="43" t="str">
         <f t="shared" si="0"/>
         <v>M1SDAWIR</v>
@@ -5362,8 +5380,8 @@
       <c r="AN12" s="104" t="s">
         <v>339</v>
       </c>
-      <c r="AO12" s="176"/>
-      <c r="AP12" s="176"/>
+      <c r="AO12" s="174"/>
+      <c r="AP12" s="174"/>
       <c r="AQ12" s="5" t="s">
         <v>349</v>
       </c>
@@ -5386,7 +5404,9 @@
       <c r="E13" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="G13" s="155"/>
+      <c r="G13" s="155" t="s">
+        <v>577</v>
+      </c>
       <c r="H13" s="43" t="str">
         <f t="shared" si="0"/>
         <v>GPIO10</v>
@@ -5460,10 +5480,10 @@
       <c r="AN13" s="105" t="s">
         <v>338</v>
       </c>
-      <c r="AO13" s="176" t="s">
+      <c r="AO13" s="174" t="s">
         <v>438</v>
       </c>
-      <c r="AP13" s="176"/>
+      <c r="AP13" s="174"/>
       <c r="AQ13" s="5" t="s">
         <v>349</v>
       </c>
@@ -5576,8 +5596,8 @@
       <c r="AN14" s="106" t="s">
         <v>348</v>
       </c>
-      <c r="AO14" s="185"/>
-      <c r="AP14" s="185"/>
+      <c r="AO14" s="190"/>
+      <c r="AP14" s="190"/>
       <c r="AQ14" s="5" t="s">
         <v>349</v>
       </c>
@@ -5599,9 +5619,6 @@
       </c>
       <c r="E15" s="43" t="s">
         <v>209</v>
-      </c>
-      <c r="G15" s="172" t="s">
-        <v>574</v>
       </c>
       <c r="H15" s="43" t="str">
         <f t="shared" si="0"/>
@@ -5692,10 +5709,10 @@
       <c r="AN15" s="107" t="s">
         <v>152</v>
       </c>
-      <c r="AO15" s="176" t="s">
+      <c r="AO15" s="174" t="s">
         <v>152</v>
       </c>
-      <c r="AP15" s="176"/>
+      <c r="AP15" s="174"/>
       <c r="AQ15" s="5" t="s">
         <v>349</v>
       </c>
@@ -5717,9 +5734,6 @@
       </c>
       <c r="E16" s="43" t="s">
         <v>207</v>
-      </c>
-      <c r="G16" s="172" t="s">
-        <v>575</v>
       </c>
       <c r="H16" s="43" t="str">
         <f t="shared" si="0"/>
@@ -5810,10 +5824,10 @@
       <c r="AN16" s="108" t="s">
         <v>158</v>
       </c>
-      <c r="AO16" s="176" t="s">
+      <c r="AO16" s="174" t="s">
         <v>158</v>
       </c>
-      <c r="AP16" s="176"/>
+      <c r="AP16" s="174"/>
       <c r="AQ16" s="5" t="s">
         <v>349</v>
       </c>
@@ -5837,7 +5851,7 @@
         <v>208</v>
       </c>
       <c r="G17" s="172" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="H17" s="43" t="str">
         <f t="shared" si="0"/>
@@ -5912,10 +5926,10 @@
       <c r="AN17" s="109" t="s">
         <v>164</v>
       </c>
-      <c r="AO17" s="176" t="s">
+      <c r="AO17" s="174" t="s">
         <v>143</v>
       </c>
-      <c r="AP17" s="176"/>
+      <c r="AP17" s="174"/>
       <c r="AQ17" s="5" t="s">
         <v>349</v>
       </c>
@@ -5939,7 +5953,7 @@
         <v>206</v>
       </c>
       <c r="G18" s="172" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="H18" s="43" t="str">
         <f t="shared" si="0"/>
@@ -6014,10 +6028,10 @@
       <c r="AN18" s="110" t="s">
         <v>356</v>
       </c>
-      <c r="AO18" s="176" t="s">
+      <c r="AO18" s="174" t="s">
         <v>144</v>
       </c>
-      <c r="AP18" s="176"/>
+      <c r="AP18" s="174"/>
       <c r="AQ18" s="5" t="s">
         <v>349</v>
       </c>
@@ -6041,7 +6055,7 @@
         <v>217</v>
       </c>
       <c r="G19" s="172" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H19" s="43" t="str">
         <f>IF(Q19="",E19,IF(J19="","",HLOOKUP(J19,$N$2:$U$56,ROW(J19)-1)))</f>
@@ -6116,10 +6130,10 @@
       <c r="AN19" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="AO19" s="176" t="s">
+      <c r="AO19" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="AP19" s="176"/>
+      <c r="AP19" s="174"/>
       <c r="AQ19" s="5" t="s">
         <v>349</v>
       </c>
@@ -6215,10 +6229,10 @@
       <c r="AN20" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="AO20" s="176" t="s">
+      <c r="AO20" s="174" t="s">
         <v>146</v>
       </c>
-      <c r="AP20" s="176"/>
+      <c r="AP20" s="174"/>
       <c r="AQ20" s="5" t="s">
         <v>349</v>
       </c>
@@ -6328,10 +6342,10 @@
       <c r="AN21" s="113" t="s">
         <v>250</v>
       </c>
-      <c r="AO21" s="176" t="s">
+      <c r="AO21" s="174" t="s">
         <v>250</v>
       </c>
-      <c r="AP21" s="176"/>
+      <c r="AP21" s="174"/>
       <c r="AQ21" s="5" t="s">
         <v>349</v>
       </c>
@@ -6444,10 +6458,10 @@
       <c r="AN22" s="114" t="s">
         <v>33</v>
       </c>
-      <c r="AO22" s="176" t="s">
+      <c r="AO22" s="174" t="s">
         <v>33</v>
       </c>
-      <c r="AP22" s="176"/>
+      <c r="AP22" s="174"/>
       <c r="AQ22" s="5" t="s">
         <v>349</v>
       </c>
@@ -6470,7 +6484,9 @@
       <c r="E23" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="G23" s="154"/>
+      <c r="G23" s="207" t="s">
+        <v>576</v>
+      </c>
       <c r="H23" s="43" t="str">
         <f t="shared" si="0"/>
         <v>SWDCK</v>
@@ -6544,10 +6560,10 @@
       <c r="AN23" s="115" t="s">
         <v>169</v>
       </c>
-      <c r="AO23" s="176" t="s">
+      <c r="AO23" s="174" t="s">
         <v>535</v>
       </c>
-      <c r="AP23" s="176"/>
+      <c r="AP23" s="174"/>
       <c r="AQ23" s="5" t="s">
         <v>443</v>
       </c>
@@ -6570,7 +6586,9 @@
       <c r="E24" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="G24" s="154"/>
+      <c r="G24" s="207" t="s">
+        <v>130</v>
+      </c>
       <c r="H24" s="43" t="str">
         <f t="shared" si="0"/>
         <v>SWDIO</v>
@@ -6644,10 +6662,10 @@
       <c r="AN24" s="116" t="s">
         <v>258</v>
       </c>
-      <c r="AO24" s="205" t="s">
+      <c r="AO24" s="188" t="s">
         <v>271</v>
       </c>
-      <c r="AP24" s="205"/>
+      <c r="AP24" s="188"/>
       <c r="AQ24" s="6" t="s">
         <v>349</v>
       </c>
@@ -6754,10 +6772,10 @@
         <v>502</v>
       </c>
       <c r="AM25" s="9"/>
-      <c r="AN25" s="206"/>
-      <c r="AO25" s="206"/>
-      <c r="AP25" s="206"/>
-      <c r="AQ25" s="206"/>
+      <c r="AN25" s="189"/>
+      <c r="AO25" s="189"/>
+      <c r="AP25" s="189"/>
+      <c r="AQ25" s="189"/>
       <c r="AR25" s="9"/>
       <c r="AS25" s="48"/>
     </row>
@@ -6865,10 +6883,10 @@
       <c r="AN26" s="117" t="s">
         <v>265</v>
       </c>
-      <c r="AO26" s="188" t="s">
+      <c r="AO26" s="193" t="s">
         <v>269</v>
       </c>
-      <c r="AP26" s="189"/>
+      <c r="AP26" s="194"/>
       <c r="AQ26" s="4" t="s">
         <v>349</v>
       </c>
@@ -7090,10 +7108,10 @@
         <v>502</v>
       </c>
       <c r="AM28" s="9"/>
-      <c r="AN28" s="190"/>
-      <c r="AO28" s="190"/>
-      <c r="AP28" s="190"/>
-      <c r="AQ28" s="190"/>
+      <c r="AN28" s="195"/>
+      <c r="AO28" s="195"/>
+      <c r="AP28" s="195"/>
+      <c r="AQ28" s="195"/>
       <c r="AR28" s="9"/>
       <c r="AS28" s="48"/>
     </row>
@@ -7201,10 +7219,10 @@
       <c r="AN29" s="121" t="s">
         <v>505</v>
       </c>
-      <c r="AO29" s="186" t="s">
+      <c r="AO29" s="191" t="s">
         <v>506</v>
       </c>
-      <c r="AP29" s="187"/>
+      <c r="AP29" s="192"/>
       <c r="AQ29" s="13" t="s">
         <v>324</v>
       </c>
@@ -7420,12 +7438,12 @@
         <v>502</v>
       </c>
       <c r="AM31" s="9"/>
-      <c r="AN31" s="199" t="s">
+      <c r="AN31" s="182" t="s">
         <v>530</v>
       </c>
-      <c r="AO31" s="200"/>
-      <c r="AP31" s="200"/>
-      <c r="AQ31" s="201"/>
+      <c r="AO31" s="183"/>
+      <c r="AP31" s="183"/>
+      <c r="AQ31" s="184"/>
       <c r="AR31" s="9"/>
       <c r="AS31" s="48"/>
     </row>
@@ -7446,7 +7464,7 @@
         <v>212</v>
       </c>
       <c r="G32" s="172" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H32" s="43" t="str">
         <f t="shared" si="0"/>
@@ -7532,10 +7550,10 @@
         <v>502</v>
       </c>
       <c r="AM32" s="9"/>
-      <c r="AN32" s="202"/>
-      <c r="AO32" s="203"/>
-      <c r="AP32" s="203"/>
-      <c r="AQ32" s="204"/>
+      <c r="AN32" s="185"/>
+      <c r="AO32" s="186"/>
+      <c r="AP32" s="186"/>
+      <c r="AQ32" s="187"/>
       <c r="AR32" s="9"/>
       <c r="AS32" s="48"/>
     </row>
@@ -7554,9 +7572,6 @@
       </c>
       <c r="E33" s="43" t="s">
         <v>224</v>
-      </c>
-      <c r="G33" s="172" t="s">
-        <v>560</v>
       </c>
       <c r="H33" s="43" t="str">
         <f t="shared" si="0"/>
@@ -7663,9 +7678,6 @@
       <c r="E34" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="G34" s="172" t="s">
-        <v>561</v>
-      </c>
       <c r="H34" s="43" t="str">
         <f t="shared" si="0"/>
         <v>UART0RX</v>
@@ -7776,7 +7788,7 @@
         <v>225</v>
       </c>
       <c r="G35" s="172" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H35" s="43" t="str">
         <f t="shared" ref="H35:H66" si="2">IF(Q35="",E35,IF(J35="","",HLOOKUP(J35,$N$2:$U$56,ROW(J35)-1)))</f>
@@ -7884,7 +7896,7 @@
         <v>226</v>
       </c>
       <c r="G36" s="172" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H36" s="43" t="str">
         <f t="shared" si="2"/>
@@ -8085,8 +8097,8 @@
       <c r="E38" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="G38" s="172" t="s">
-        <v>573</v>
+      <c r="G38" s="1" t="s">
+        <v>575</v>
       </c>
       <c r="H38" s="43" t="str">
         <f t="shared" si="2"/>
@@ -9428,7 +9440,7 @@
         <v>245</v>
       </c>
       <c r="G51" s="172" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H51" s="43" t="str">
         <f t="shared" si="2"/>
@@ -9538,7 +9550,7 @@
         <v>246</v>
       </c>
       <c r="G52" s="172" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H52" s="43" t="str">
         <f t="shared" si="2"/>
@@ -11651,7 +11663,7 @@
       <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A87" s="191" t="s">
+      <c r="A87" s="173" t="s">
         <v>549</v>
       </c>
       <c r="B87" s="158"/>
@@ -11661,7 +11673,7 @@
       </c>
     </row>
     <row r="88" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A88" s="191"/>
+      <c r="A88" s="173"/>
       <c r="B88" s="159"/>
       <c r="D88" s="1"/>
       <c r="E88" s="165" t="s">
@@ -11669,7 +11681,7 @@
       </c>
     </row>
     <row r="89" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A89" s="191"/>
+      <c r="A89" s="173"/>
       <c r="B89" s="160"/>
       <c r="D89" s="1"/>
       <c r="E89" s="166" t="s">
@@ -11677,7 +11689,7 @@
       </c>
     </row>
     <row r="90" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A90" s="191"/>
+      <c r="A90" s="173"/>
       <c r="B90" s="161"/>
       <c r="D90" s="1"/>
       <c r="E90" s="167" t="s">
@@ -11685,7 +11697,7 @@
       </c>
     </row>
     <row r="91" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A91" s="191"/>
+      <c r="A91" s="173"/>
       <c r="B91" s="162"/>
       <c r="D91" s="1"/>
       <c r="E91" s="168" t="s">
@@ -11693,7 +11705,7 @@
       </c>
     </row>
     <row r="92" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A92" s="191"/>
+      <c r="A92" s="173"/>
       <c r="B92" s="163"/>
       <c r="D92" s="1"/>
       <c r="E92" s="169" t="s">
@@ -11871,6 +11883,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="32">
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="AO9:AP9"/>
+    <mergeCell ref="AO10:AP10"/>
+    <mergeCell ref="AO11:AP11"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="AO7:AP7"/>
+    <mergeCell ref="AN3:AQ3"/>
+    <mergeCell ref="AO14:AP14"/>
+    <mergeCell ref="AO15:AP15"/>
+    <mergeCell ref="AO17:AP17"/>
+    <mergeCell ref="AO20:AP20"/>
+    <mergeCell ref="AO29:AP29"/>
+    <mergeCell ref="AO26:AP26"/>
+    <mergeCell ref="AN28:AQ28"/>
     <mergeCell ref="A87:A92"/>
     <mergeCell ref="AO19:AP19"/>
     <mergeCell ref="AO18:AP18"/>
@@ -11887,91 +11915,75 @@
     <mergeCell ref="AN25:AQ25"/>
     <mergeCell ref="AO12:AP12"/>
     <mergeCell ref="AO13:AP13"/>
-    <mergeCell ref="AO14:AP14"/>
-    <mergeCell ref="AO15:AP15"/>
-    <mergeCell ref="AO17:AP17"/>
-    <mergeCell ref="AO20:AP20"/>
-    <mergeCell ref="AO29:AP29"/>
-    <mergeCell ref="AO26:AP26"/>
-    <mergeCell ref="AN28:AQ28"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="AO9:AP9"/>
-    <mergeCell ref="AO10:AP10"/>
-    <mergeCell ref="AO11:AP11"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="AO7:AP7"/>
-    <mergeCell ref="AN3:AQ3"/>
   </mergeCells>
   <conditionalFormatting sqref="N3:U83">
-    <cfRule type="expression" dxfId="23" priority="4574">
+    <cfRule type="expression" dxfId="23" priority="4571">
+      <formula>AND(IF($V3="",1),IF(LEFT($AQ$24,1)="N",1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="4572">
+      <formula>AND(IF(LEFT(N3,3)="NCE",1),IF(LEFT($AQ$13,1)="N",1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="4573">
+      <formula>AND(IF(LEFT(N3,3)="SCC",1),IF(LEFT($AQ$14,1)="N",1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="4574">
       <formula>AND(OR(IF(LEFT(N3,3)="BLE",1),IF(RIGHT(N3,2)="LB",1),IF(RIGHT(N3,2)="GP",1),IF(LEFT(N3,3)="EXT",1),IF(LEFT(N3,7)="ANATEST",1)),IF(LEFT($AQ$23,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="4584">
-      <formula>IF($J3="",0,AND(IF($J3=N$2,1),IF(LEFT($AQ$26,1)="Y",1)))</formula>
+    <cfRule type="expression" dxfId="19" priority="4575">
+      <formula>AND(OR(IF(LEFT(N3,6)="GPIO03",1),IF(LEFT(N3,6)="GPIO36",1),IF(LEFT(N3,6)="GPIO37",1),IF(LEFT(N3,6)="GPIO41",1)),IF(LEFT($AQ$20,1)="Y",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="4583">
-      <formula>AND(IF(LEFT(N3,2)="SL",1),IF(LEFT($AQ$5,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="18" priority="4576">
+      <formula>AND(IF(LEFT(N3,2)="SW",1),IF(LEFT($AQ$22,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="4582">
-      <formula>AND(OR(IF(LEFT(N3,3)="UA0",1),IF(LEFT(N3,5)="UART0",1)),IF(LEFT($AQ$15,1)="N",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4581">
-      <formula>AND(OR(IF(LEFT(N3,3)="UA1",1),IF(LEFT(N3,5)="UART1",1)),IF(LEFT($AQ$16,1)="N",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4580">
-      <formula>AND(OR(IF(LEFT(N3,3)="ADC",1),IF(LEFT(N3,3)="CMP",1),IF(LEFT(N3,4)="TRIG",1)),IF(LEFT($AQ$17,1)="N",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="4579">
-      <formula>AND(IF(LEFT(N3,2)="CT",1),IF(LEFT($AQ$18,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="17" priority="4577">
+      <formula>AND(OR(IF(LEFT(N3,3)="CLK",1),IF(LEFT(N3,3)="32K",1)),IF(LEFT($AQ$19,1)="N",1))</formula>
     </cfRule>
     <cfRule type="expression" dxfId="16" priority="4578">
       <formula>AND(OR(IF(LEFT(N3,3)="I2S",1),IF(LEFT(N3,3)="PDM",1)),IF(LEFT($AQ$21,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4577">
-      <formula>AND(OR(IF(LEFT(N3,3)="CLK",1),IF(LEFT(N3,3)="32K",1)),IF(LEFT($AQ$19,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="15" priority="4579">
+      <formula>AND(IF(LEFT(N3,2)="CT",1),IF(LEFT($AQ$18,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="4571">
-      <formula>AND(IF($V3="",1),IF(LEFT($AQ$24,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="14" priority="4580">
+      <formula>AND(OR(IF(LEFT(N3,3)="ADC",1),IF(LEFT(N3,3)="CMP",1),IF(LEFT(N3,4)="TRIG",1)),IF(LEFT($AQ$17,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4572">
-      <formula>AND(IF(LEFT(N3,3)="NCE",1),IF(LEFT($AQ$13,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="13" priority="4581">
+      <formula>AND(OR(IF(LEFT(N3,3)="UA1",1),IF(LEFT(N3,5)="UART1",1)),IF(LEFT($AQ$16,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="4573">
-      <formula>AND(IF(LEFT(N3,3)="SCC",1),IF(LEFT($AQ$14,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="12" priority="4582">
+      <formula>AND(OR(IF(LEFT(N3,3)="UA0",1),IF(LEFT(N3,5)="UART0",1)),IF(LEFT($AQ$15,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4585">
+    <cfRule type="expression" dxfId="11" priority="4583">
+      <formula>AND(IF(LEFT(N3,2)="SL",1),IF(LEFT($AQ$5,1)="N",1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="4584">
+      <formula>IF($J3="",0,AND(IF($J3=N$2,1),IF(LEFT($AQ$26,1)="Y",1)))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="4585">
       <formula>AND(IF($J3=N$2,0,1),IF($J3="",0,1),IF(LEFT($AQ$27,1)="Y",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="4575">
-      <formula>AND(OR(IF(LEFT(N3,6)="GPIO03",1),IF(LEFT(N3,6)="GPIO36",1),IF(LEFT(N3,6)="GPIO37",1),IF(LEFT(N3,6)="GPIO41",1)),IF(LEFT($AQ$20,1)="Y",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4576">
-      <formula>AND(IF(LEFT(N3,2)="SW",1),IF(LEFT($AQ$22,1)="N",1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:V52 X3:AB52 N53:AB83 X55:AR83">
-    <cfRule type="expression" dxfId="8" priority="3509">
+    <cfRule type="expression" dxfId="8" priority="3506">
+      <formula>AND(IF(LEFT(N3,2)="M5",1),IF(LEFT($AQ$11,1)="N",1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="3507">
+      <formula>AND(IF(LEFT(N3,2)="M4",1),IF(LEFT($AQ$10,1)="N",1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="3508">
+      <formula>AND(IF(LEFT(N3,2)="M3",1),IF(LEFT($AQ$9,1)="N",1))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3509">
       <formula>AND(IF(LEFT(N3,2)="M2",1),IF(LEFT($AQ$8,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3512">
-      <formula>AND(IF(LEFT(N3,4)="MSPI",1),IF(LEFT($AQ$12,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="4" priority="3510">
+      <formula>AND(IF(LEFT(N3,2)="M1",1),IF(LEFT($AQ$7,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3511">
+    <cfRule type="expression" dxfId="3" priority="3511">
       <formula>AND(IF(LEFT(N3,2)="M0",1),IF(LEFT($AQ$6,1)="N",1))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3510">
-      <formula>AND(IF(LEFT(N3,2)="M1",1),IF(LEFT($AQ$7,1)="N",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3506">
-      <formula>AND(IF(LEFT(N3,2)="M5",1),IF(LEFT($AQ$11,1)="N",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3508">
-      <formula>AND(IF(LEFT(N3,2)="M3",1),IF(LEFT($AQ$9,1)="N",1))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3507">
-      <formula>AND(IF(LEFT(N3,2)="M4",1),IF(LEFT($AQ$10,1)="N",1))</formula>
+    <cfRule type="expression" dxfId="2" priority="3512">
+      <formula>AND(IF(LEFT(N3,4)="MSPI",1),IF(LEFT($AQ$12,1)="N",1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W52">

</xml_diff>